<commit_message>
dw dim and fact table creation
</commit_message>
<xml_diff>
--- a/ETL+DW/DW_Assignments_Day1.xlsx
+++ b/ETL+DW/DW_Assignments_Day1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
   <si>
     <t>Dim_Customer</t>
   </si>
@@ -166,6 +166,12 @@
   </si>
   <si>
     <t>Dimension and Fact tables on MMT One way flight booking System</t>
+  </si>
+  <si>
+    <t>Booking_amount</t>
+  </si>
+  <si>
+    <t>Refund_amount</t>
   </si>
 </sst>
 </file>
@@ -342,7 +348,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -364,6 +370,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -660,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -978,20 +986,34 @@
         <v>32</v>
       </c>
       <c r="C34" s="11"/>
-      <c r="F34" s="12" t="s">
+      <c r="F34" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="16"/>
-      <c r="K34" s="13"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="11"/>
     </row>
     <row r="35" spans="2:11">
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C35" s="11"/>
+      <c r="F35" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="16"/>
+      <c r="K35" s="13"/>
+    </row>
+    <row r="36" spans="2:11">
+      <c r="B36" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="13"/>
+      <c r="C36" s="13"/>
     </row>
     <row r="40" spans="2:11">
       <c r="B40" s="20" t="s">

</xml_diff>